<commit_message>
Format gridlines for all grpahs
</commit_message>
<xml_diff>
--- a/excel/cars-sample.xlsx
+++ b/excel/cars-sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mollywirtz/Documents/Classes/CS 4802 - BioVis/a2/02-DataVis-5Ways/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E424DCAA-E98F-6541-ABD5-E048B0241202}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA43C43-A406-CF47-9AE5-84D7BA6A0526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51100" yWindow="620" windowWidth="20900" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48940" yWindow="520" windowWidth="23060" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
@@ -601,11 +601,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFECECEC"/>
+      <color rgb="FF4EBC8C"/>
       <color rgb="FF33ADEB"/>
       <color rgb="FFE46962"/>
       <color rgb="FFA9AA4B"/>
       <color rgb="FFDC78E3"/>
-      <color rgb="FF4EBC8C"/>
       <color rgb="FFF65F5C"/>
     </mruColors>
   </colors>
@@ -1778,12 +1779,9 @@
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="bg1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1898,12 +1896,9 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="bg1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1912,9 +1907,12 @@
         </c:majorGridlines>
         <c:minorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:round/>
+            <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -2015,9 +2013,12 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
+        <c:minorUnit val="5"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:srgbClr val="ECECEC"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -2036,9 +2037,7 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
+    <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="tx1">
@@ -5084,7 +5083,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{2918BE99-BE2F-3B46-B5B2-10F895B7133D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>